<commit_message>
Anonymised most tests, all tests passing.
</commit_message>
<xml_diff>
--- a/src/test/resources/devils_burdens/dead_heats/master.xlsx
+++ b/src/test/resources/devils_burdens/dead_heats/master.xlsx
@@ -80,7 +80,7 @@
     <t>Leg 4</t>
   </si>
   <si>
-    <t>Anster Haddies Ladies B</t>
+    <t>Team 1</t>
   </si>
   <si>
     <t>Women Senior</t>
@@ -98,7 +98,7 @@
     <t>Rosie Knox</t>
   </si>
   <si>
-    <t>Anster Haddies Mens 1</t>
+    <t>Team 2</t>
   </si>
   <si>
     <t>Open 50+</t>

</xml_diff>